<commit_message>
Resultados - Modelo Computacional
</commit_message>
<xml_diff>
--- a/Resources/Excel/Celulas de Carga.xlsx
+++ b/Resources/Excel/Celulas de Carga.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="20025"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="20025" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CelulaComercial5Kg" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Tensão (V)</t>
   </si>
@@ -80,6 +80,15 @@
   </si>
   <si>
     <t>mV</t>
+  </si>
+  <si>
+    <t>M pela FT</t>
+  </si>
+  <si>
+    <t>Erro regressão</t>
+  </si>
+  <si>
+    <t>m pela FT</t>
   </si>
 </sst>
 </file>
@@ -607,11 +616,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="480554056"/>
-        <c:axId val="480557584"/>
+        <c:axId val="416233216"/>
+        <c:axId val="416237528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="480554056"/>
+        <c:axId val="416233216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -668,12 +677,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="480557584"/>
+        <c:crossAx val="416237528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="480557584"/>
+        <c:axId val="416237528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -730,7 +739,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="480554056"/>
+        <c:crossAx val="416233216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1005,11 +1014,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="480557192"/>
-        <c:axId val="480559936"/>
+        <c:axId val="413675400"/>
+        <c:axId val="413675008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="480557192"/>
+        <c:axId val="413675400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1066,12 +1075,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="480559936"/>
+        <c:crossAx val="413675008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="480559936"/>
+        <c:axId val="413675008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1128,7 +1137,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="480557192"/>
+        <c:crossAx val="413675400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1367,11 +1376,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="480560328"/>
-        <c:axId val="480561504"/>
+        <c:axId val="413672656"/>
+        <c:axId val="413677752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="480560328"/>
+        <c:axId val="413672656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1428,12 +1437,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="480561504"/>
+        <c:crossAx val="413677752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="480561504"/>
+        <c:axId val="413677752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1490,7 +1499,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="480560328"/>
+        <c:crossAx val="413672656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3246,16 +3255,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>319087</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>465625</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>129319</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>14287</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>160825</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>15019</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3577,13 +3586,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I53" sqref="I2:I53"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -3599,6 +3609,12 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -3611,9 +3627,13 @@
         <f>CONCATENATE("{", A2, ",", B2, "},")</f>
         <v>{0,1.899},</v>
       </c>
-      <c r="I2">
-        <f t="shared" ref="I2:I52" si="0">B2/29.2424</f>
-        <v>6.4939950209285155E-2</v>
+      <c r="H2">
+        <f>32.9198-(17.3681*B2)</f>
+        <v>-6.2221899999997277E-2</v>
+      </c>
+      <c r="I2" s="3" t="e">
+        <f>((A2-H2)/A2)*100</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -3624,15 +3644,19 @@
         <v>1.887</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C52" si="1">CONCATENATE("{", A3, ",", B3, "},")</f>
+        <f t="shared" ref="C3:C52" si="0">CONCATENATE("{", A3, ",", B3, "},")</f>
         <v>{0.2,1.887},</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="I3">
-        <f t="shared" si="0"/>
-        <v>6.4529587174787295E-2</v>
+      <c r="H3">
+        <f t="shared" ref="H3:H53" si="1">32.9198-(17.3681*B3)</f>
+        <v>0.14619530000000225</v>
+      </c>
+      <c r="I3" s="3">
+        <f t="shared" ref="I3:I53" si="2">((A3-H3)/A3)*100</f>
+        <v>26.902349999998883</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -3643,7 +3667,7 @@
         <v>1.875</v>
       </c>
       <c r="C4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{0.4,1.875},</v>
       </c>
       <c r="D4" t="s">
@@ -3652,9 +3676,13 @@
       <c r="E4" t="s">
         <v>9</v>
       </c>
-      <c r="I4">
-        <f t="shared" si="0"/>
-        <v>6.4119224140289449E-2</v>
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>0.35461250000000888</v>
+      </c>
+      <c r="I4" s="3">
+        <f t="shared" si="2"/>
+        <v>11.346874999997786</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -3665,15 +3693,19 @@
         <v>1.863</v>
       </c>
       <c r="C5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{0.6,1.863},</v>
       </c>
       <c r="E5" t="s">
         <v>6</v>
       </c>
-      <c r="I5">
-        <f t="shared" si="0"/>
-        <v>6.3708861105791589E-2</v>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>0.5630297000000084</v>
+      </c>
+      <c r="I5" s="3">
+        <f t="shared" si="2"/>
+        <v>6.1617166666652619</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -3684,7 +3716,7 @@
         <v>1.8520000000000001</v>
       </c>
       <c r="C6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{0.8,1.852},</v>
       </c>
       <c r="E6" t="s">
@@ -3693,9 +3725,13 @@
       <c r="G6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I6">
-        <f t="shared" si="0"/>
-        <v>6.3332694990835228E-2</v>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>0.75407880000000205</v>
+      </c>
+      <c r="I6" s="3">
+        <f t="shared" si="2"/>
+        <v>5.7401499999997494</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -3706,12 +3742,16 @@
         <v>1.841</v>
       </c>
       <c r="C7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{1,1.841},</v>
       </c>
-      <c r="I7">
-        <f t="shared" si="0"/>
-        <v>6.2956528875878853E-2</v>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>0.94512790000000635</v>
+      </c>
+      <c r="I7" s="3">
+        <f t="shared" si="2"/>
+        <v>5.4872099999993651</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -3722,12 +3762,16 @@
         <v>1.823</v>
       </c>
       <c r="C8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{1.2,1.823},</v>
       </c>
-      <c r="I8">
-        <f t="shared" si="0"/>
-        <v>6.2340984324132077E-2</v>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>1.2577537000000056</v>
+      </c>
+      <c r="I8" s="3">
+        <f t="shared" si="2"/>
+        <v>-4.8128083333338072</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -3738,12 +3782,16 @@
         <v>1.8180000000000001</v>
       </c>
       <c r="C9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{1.4,1.818},</v>
       </c>
-      <c r="I9">
-        <f t="shared" si="0"/>
-        <v>6.2169999726424646E-2</v>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>1.3445942000000031</v>
+      </c>
+      <c r="I9" s="3">
+        <f t="shared" si="2"/>
+        <v>3.9575571428569178</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -3754,12 +3802,16 @@
         <v>1.806</v>
       </c>
       <c r="C10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{1.6,1.806},</v>
       </c>
-      <c r="I10">
-        <f t="shared" si="0"/>
-        <v>6.1759636691926793E-2</v>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>1.5530114000000026</v>
+      </c>
+      <c r="I10" s="3">
+        <f t="shared" si="2"/>
+        <v>2.9367874999998431</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -3770,12 +3822,16 @@
         <v>1.7949999999999999</v>
       </c>
       <c r="C11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{1.8,1.795},</v>
       </c>
-      <c r="I11">
-        <f t="shared" si="0"/>
-        <v>6.1383470576970425E-2</v>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>1.7440605000000069</v>
+      </c>
+      <c r="I11" s="3">
+        <f t="shared" si="2"/>
+        <v>3.1077499999996192</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -3786,12 +3842,16 @@
         <v>1.784</v>
       </c>
       <c r="C12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{2,1.784},</v>
       </c>
-      <c r="I12">
-        <f t="shared" si="0"/>
-        <v>6.1007304462014064E-2</v>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>1.9351096000000041</v>
+      </c>
+      <c r="I12" s="3">
+        <f t="shared" si="2"/>
+        <v>3.2445199999997953</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -3802,12 +3862,16 @@
         <v>1.766</v>
       </c>
       <c r="C13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{2.2,1.766},</v>
       </c>
-      <c r="I13">
-        <f t="shared" si="0"/>
-        <v>6.0391759910267281E-2</v>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>2.2477354000000034</v>
+      </c>
+      <c r="I13" s="3">
+        <f t="shared" si="2"/>
+        <v>-2.1697909090910543</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -3818,12 +3882,16 @@
         <v>1.76</v>
       </c>
       <c r="C14" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{2.4,1.76},</v>
       </c>
-      <c r="I14">
-        <f t="shared" si="0"/>
-        <v>6.0186578393018358E-2</v>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>2.3519440000000067</v>
+      </c>
+      <c r="I14" s="3">
+        <f t="shared" si="2"/>
+        <v>2.0023333333330506</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -3834,12 +3902,16 @@
         <v>1.748</v>
       </c>
       <c r="C15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{2.6,1.748},</v>
       </c>
-      <c r="I15">
-        <f t="shared" si="0"/>
-        <v>5.9776215358520506E-2</v>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>2.5603612000000062</v>
+      </c>
+      <c r="I15" s="3">
+        <f t="shared" si="2"/>
+        <v>1.5245692307689949</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -3850,12 +3922,16 @@
         <v>1.7370000000000001</v>
       </c>
       <c r="C16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{2.8,1.737},</v>
       </c>
-      <c r="I16">
-        <f t="shared" si="0"/>
-        <v>5.9400049243564144E-2</v>
+      <c r="H16">
+        <f t="shared" si="1"/>
+        <v>2.7514103000000034</v>
+      </c>
+      <c r="I16" s="3">
+        <f t="shared" si="2"/>
+        <v>1.7353464285713005</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -3866,12 +3942,16 @@
         <v>1.724</v>
       </c>
       <c r="C17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{3,1.724},</v>
       </c>
-      <c r="I17">
-        <f t="shared" si="0"/>
-        <v>5.89554892895248E-2</v>
+      <c r="H17">
+        <f t="shared" si="1"/>
+        <v>2.9771956000000053</v>
+      </c>
+      <c r="I17" s="3">
+        <f t="shared" si="2"/>
+        <v>0.76014666666649089</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -3882,12 +3962,16 @@
         <v>1.708</v>
       </c>
       <c r="C18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{3.2,1.708},</v>
       </c>
-      <c r="I18">
-        <f t="shared" si="0"/>
-        <v>5.8408338576860994E-2</v>
+      <c r="H18">
+        <f t="shared" si="1"/>
+        <v>3.255085200000007</v>
+      </c>
+      <c r="I18" s="3">
+        <f t="shared" si="2"/>
+        <v>-1.7214125000002134</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -3898,12 +3982,16 @@
         <v>1.702</v>
       </c>
       <c r="C19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{3.4,1.702},</v>
       </c>
-      <c r="I19">
-        <f t="shared" si="0"/>
-        <v>5.8203157059612071E-2</v>
+      <c r="H19">
+        <f t="shared" si="1"/>
+        <v>3.3592938000000068</v>
+      </c>
+      <c r="I19" s="3">
+        <f t="shared" si="2"/>
+        <v>1.1972411764703865</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -3914,12 +4002,16 @@
         <v>1.6910000000000001</v>
       </c>
       <c r="C20" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{3.6,1.691},</v>
       </c>
-      <c r="I20">
-        <f t="shared" si="0"/>
-        <v>5.782699094465571E-2</v>
+      <c r="H20">
+        <f t="shared" si="1"/>
+        <v>3.550342900000004</v>
+      </c>
+      <c r="I20" s="3">
+        <f t="shared" si="2"/>
+        <v>1.3793638888887811</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -3930,12 +4022,16 @@
         <v>1.679</v>
       </c>
       <c r="C21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{3.8,1.679},</v>
       </c>
-      <c r="I21">
-        <f t="shared" si="0"/>
-        <v>5.7416627910157857E-2</v>
+      <c r="H21">
+        <f t="shared" si="1"/>
+        <v>3.7587601000000035</v>
+      </c>
+      <c r="I21" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0852605263156929</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -3946,12 +4042,16 @@
         <v>1.6679999999999999</v>
       </c>
       <c r="C22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{4,1.668},</v>
       </c>
-      <c r="I22">
-        <f t="shared" si="0"/>
-        <v>5.7040461795201489E-2</v>
+      <c r="H22">
+        <f t="shared" si="1"/>
+        <v>3.9498092000000078</v>
+      </c>
+      <c r="I22" s="3">
+        <f t="shared" si="2"/>
+        <v>1.2547699999998052</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -3962,12 +4062,16 @@
         <v>1.6519999999999999</v>
       </c>
       <c r="C23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{4.2,1.652},</v>
       </c>
-      <c r="I23">
-        <f t="shared" si="0"/>
-        <v>5.6493311082537682E-2</v>
+      <c r="H23">
+        <f t="shared" si="1"/>
+        <v>4.227698800000006</v>
+      </c>
+      <c r="I23" s="3">
+        <f t="shared" si="2"/>
+        <v>-0.65949523809537614</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -3978,12 +4082,16 @@
         <v>1.6439999999999999</v>
       </c>
       <c r="C24" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{4.4,1.644},</v>
       </c>
-      <c r="I24">
-        <f t="shared" si="0"/>
-        <v>5.6219735726205783E-2</v>
+      <c r="H24">
+        <f t="shared" si="1"/>
+        <v>4.3666436000000068</v>
+      </c>
+      <c r="I24" s="3">
+        <f t="shared" si="2"/>
+        <v>0.75809999999985256</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -3994,12 +4102,16 @@
         <v>1.631</v>
       </c>
       <c r="C25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{4.6,1.631},</v>
       </c>
-      <c r="I25">
-        <f t="shared" si="0"/>
-        <v>5.5775175772166445E-2</v>
+      <c r="H25">
+        <f t="shared" si="1"/>
+        <v>4.5924289000000051</v>
+      </c>
+      <c r="I25" s="3">
+        <f t="shared" si="2"/>
+        <v>0.16458913043466308</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -4010,12 +4122,16 @@
         <v>1.621</v>
       </c>
       <c r="C26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{4.8,1.621},</v>
       </c>
-      <c r="I26">
-        <f t="shared" si="0"/>
-        <v>5.5433206576751569E-2</v>
+      <c r="H26">
+        <f t="shared" si="1"/>
+        <v>4.7661099000000036</v>
+      </c>
+      <c r="I26" s="3">
+        <f t="shared" si="2"/>
+        <v>0.70604374999992214</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -4026,12 +4142,16 @@
         <v>1.609</v>
       </c>
       <c r="C27" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{5,1.609},</v>
       </c>
-      <c r="I27">
-        <f t="shared" si="0"/>
-        <v>5.5022843542253716E-2</v>
+      <c r="H27">
+        <f t="shared" si="1"/>
+        <v>4.9745271000000066</v>
+      </c>
+      <c r="I27" s="3">
+        <f t="shared" si="2"/>
+        <v>0.50945799999986718</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -4042,12 +4162,16 @@
         <v>1.8959999999999999</v>
       </c>
       <c r="C28" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{0,1.896},</v>
       </c>
-      <c r="I28">
-        <f t="shared" si="0"/>
-        <v>6.4837359450660687E-2</v>
+      <c r="H28">
+        <f t="shared" si="1"/>
+        <v>-1.0117599999993843E-2</v>
+      </c>
+      <c r="I28" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -4058,12 +4182,16 @@
         <v>1.885</v>
       </c>
       <c r="C29" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{0.2,1.885},</v>
       </c>
-      <c r="I29">
-        <f t="shared" si="0"/>
-        <v>6.4461193335704325E-2</v>
+      <c r="H29">
+        <f t="shared" si="1"/>
+        <v>0.18093150000000691</v>
+      </c>
+      <c r="I29" s="3">
+        <f t="shared" si="2"/>
+        <v>9.5342499999965522</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -4074,12 +4202,16 @@
         <v>1.867</v>
       </c>
       <c r="C30" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{0.4,1.867},</v>
       </c>
-      <c r="I30">
-        <f t="shared" si="0"/>
-        <v>6.3845648783957543E-2</v>
+      <c r="H30">
+        <f t="shared" si="1"/>
+        <v>0.49355730000000619</v>
+      </c>
+      <c r="I30" s="3">
+        <f t="shared" si="2"/>
+        <v>-23.389325000001541</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -4090,12 +4222,16 @@
         <v>1.8580000000000001</v>
       </c>
       <c r="C31" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{0.6,1.858},</v>
       </c>
-      <c r="I31">
-        <f t="shared" si="0"/>
-        <v>6.3537876508084151E-2</v>
+      <c r="H31">
+        <f t="shared" si="1"/>
+        <v>0.64987020000000228</v>
+      </c>
+      <c r="I31" s="3">
+        <f t="shared" si="2"/>
+        <v>-8.3117000000003856</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -4106,12 +4242,16 @@
         <v>1.8460000000000001</v>
       </c>
       <c r="C32" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{0.8,1.846},</v>
       </c>
-      <c r="I32">
-        <f t="shared" si="0"/>
-        <v>6.3127513473586305E-2</v>
+      <c r="H32">
+        <f t="shared" si="1"/>
+        <v>0.85828740000000181</v>
+      </c>
+      <c r="I32" s="3">
+        <f t="shared" si="2"/>
+        <v>-7.2859250000002209</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -4122,12 +4262,16 @@
         <v>1.8340000000000001</v>
       </c>
       <c r="C33" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{1,1.834},</v>
       </c>
-      <c r="I33">
-        <f t="shared" si="0"/>
-        <v>6.2717150439088445E-2</v>
+      <c r="H33">
+        <f t="shared" si="1"/>
+        <v>1.0667046000000049</v>
+      </c>
+      <c r="I33" s="3">
+        <f t="shared" si="2"/>
+        <v>-6.6704600000004888</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -4138,12 +4282,16 @@
         <v>1.827</v>
       </c>
       <c r="C34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{1.2,1.827},</v>
       </c>
-      <c r="I34">
-        <f t="shared" si="0"/>
-        <v>6.2477772002298031E-2</v>
+      <c r="H34">
+        <f t="shared" si="1"/>
+        <v>1.188281300000007</v>
+      </c>
+      <c r="I34" s="3">
+        <f t="shared" si="2"/>
+        <v>0.97655833333274811</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -4154,12 +4302,16 @@
         <v>1.8109999999999999</v>
       </c>
       <c r="C35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{1.4,1.811},</v>
       </c>
-      <c r="I35">
-        <f t="shared" si="0"/>
-        <v>6.1930621289634225E-2</v>
+      <c r="H35">
+        <f t="shared" si="1"/>
+        <v>1.4661709000000052</v>
+      </c>
+      <c r="I35" s="3">
+        <f t="shared" si="2"/>
+        <v>-4.7264928571432323</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -4170,12 +4322,16 @@
         <v>1.7989999999999999</v>
       </c>
       <c r="C36" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{1.6,1.799},</v>
       </c>
-      <c r="I36">
-        <f t="shared" si="0"/>
-        <v>6.1520258255136379E-2</v>
+      <c r="H36">
+        <f t="shared" si="1"/>
+        <v>1.6745881000000047</v>
+      </c>
+      <c r="I36" s="3">
+        <f t="shared" si="2"/>
+        <v>-4.6617562500002876</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -4186,12 +4342,16 @@
         <v>1.788</v>
       </c>
       <c r="C37" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{1.8,1.788},</v>
       </c>
-      <c r="I37">
-        <f t="shared" si="0"/>
-        <v>6.1144092140180011E-2</v>
+      <c r="H37">
+        <f t="shared" si="1"/>
+        <v>1.8656372000000054</v>
+      </c>
+      <c r="I37" s="3">
+        <f t="shared" si="2"/>
+        <v>-3.6465111111114106</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -4202,12 +4362,16 @@
         <v>1.7809999999999999</v>
       </c>
       <c r="C38" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{2,1.781},</v>
       </c>
-      <c r="I38">
-        <f t="shared" si="0"/>
-        <v>6.0904713703389596E-2</v>
+      <c r="H38">
+        <f t="shared" si="1"/>
+        <v>1.9872139000000075</v>
+      </c>
+      <c r="I38" s="3">
+        <f t="shared" si="2"/>
+        <v>0.63930499999962365</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -4218,12 +4382,16 @@
         <v>1.7689999999999999</v>
       </c>
       <c r="C39" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{2.2,1.769},</v>
       </c>
-      <c r="I39">
-        <f t="shared" si="0"/>
-        <v>6.0494350668891743E-2</v>
+      <c r="H39">
+        <f t="shared" si="1"/>
+        <v>2.1956311000000071</v>
+      </c>
+      <c r="I39" s="3">
+        <f t="shared" si="2"/>
+        <v>0.19858636363605117</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -4234,12 +4402,16 @@
         <v>1.7569999999999999</v>
       </c>
       <c r="C40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{2.4,1.757},</v>
       </c>
-      <c r="I40">
-        <f t="shared" si="0"/>
-        <v>6.008398763439389E-2</v>
+      <c r="H40">
+        <f t="shared" si="1"/>
+        <v>2.4040483000000066</v>
+      </c>
+      <c r="I40" s="3">
+        <f t="shared" si="2"/>
+        <v>-0.16867916666694444</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -4250,12 +4422,16 @@
         <v>1.7430000000000001</v>
       </c>
       <c r="C41" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{2.6,1.743},</v>
       </c>
-      <c r="I41">
-        <f t="shared" si="0"/>
-        <v>5.9605230760813067E-2</v>
+      <c r="H41">
+        <f t="shared" si="1"/>
+        <v>2.6472017000000037</v>
+      </c>
+      <c r="I41" s="3">
+        <f t="shared" si="2"/>
+        <v>-1.815450000000137</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -4266,12 +4442,16 @@
         <v>1.734</v>
       </c>
       <c r="C42" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{2.8,1.734},</v>
       </c>
-      <c r="I42">
-        <f t="shared" si="0"/>
-        <v>5.9297458484939676E-2</v>
+      <c r="H42">
+        <f t="shared" si="1"/>
+        <v>2.8035146000000069</v>
+      </c>
+      <c r="I42" s="3">
+        <f t="shared" si="2"/>
+        <v>-0.12552142857167961</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -4282,12 +4462,16 @@
         <v>1.718</v>
       </c>
       <c r="C43" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{3,1.718},</v>
       </c>
-      <c r="I43">
-        <f t="shared" si="0"/>
-        <v>5.875030777227587E-2</v>
+      <c r="H43">
+        <f t="shared" si="1"/>
+        <v>3.081404200000005</v>
+      </c>
+      <c r="I43" s="3">
+        <f t="shared" si="2"/>
+        <v>-2.7134733333335008</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -4298,12 +4482,16 @@
         <v>1.712</v>
       </c>
       <c r="C44" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{3.2,1.712},</v>
       </c>
-      <c r="I44">
-        <f t="shared" si="0"/>
-        <v>5.8545126255026947E-2</v>
+      <c r="H44">
+        <f t="shared" si="1"/>
+        <v>3.1856128000000048</v>
+      </c>
+      <c r="I44" s="3">
+        <f t="shared" si="2"/>
+        <v>0.44959999999985567</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -4314,12 +4502,16 @@
         <v>1.6950000000000001</v>
       </c>
       <c r="C45" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{3.4,1.695},</v>
       </c>
-      <c r="I45">
-        <f t="shared" si="0"/>
-        <v>5.7963778622821656E-2</v>
+      <c r="H45">
+        <f t="shared" si="1"/>
+        <v>3.4808705000000053</v>
+      </c>
+      <c r="I45" s="3">
+        <f t="shared" si="2"/>
+        <v>-2.3785441176472175</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -4330,12 +4522,16 @@
         <v>1.6839999999999999</v>
       </c>
       <c r="C46" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{3.6,1.684},</v>
       </c>
-      <c r="I46">
-        <f t="shared" si="0"/>
-        <v>5.7587612507865288E-2</v>
+      <c r="H46">
+        <f t="shared" si="1"/>
+        <v>3.6719196000000061</v>
+      </c>
+      <c r="I46" s="3">
+        <f t="shared" si="2"/>
+        <v>-1.9977666666668323</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -4346,12 +4542,16 @@
         <v>1.671</v>
       </c>
       <c r="C47" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{3.8,1.671},</v>
       </c>
-      <c r="I47">
-        <f t="shared" si="0"/>
-        <v>5.714305255382595E-2</v>
+      <c r="H47">
+        <f t="shared" si="1"/>
+        <v>3.8977049000000044</v>
+      </c>
+      <c r="I47" s="3">
+        <f t="shared" si="2"/>
+        <v>-2.5711815789474879</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -4362,12 +4562,16 @@
         <v>1.665</v>
       </c>
       <c r="C48" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{4,1.665},</v>
       </c>
-      <c r="I48">
-        <f t="shared" si="0"/>
-        <v>5.6937871036577027E-2</v>
+      <c r="H48">
+        <f t="shared" si="1"/>
+        <v>4.0019135000000041</v>
+      </c>
+      <c r="I48" s="3">
+        <f t="shared" si="2"/>
+        <v>-4.7837500000103006E-2</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -4378,12 +4582,16 @@
         <v>1.6539999999999999</v>
       </c>
       <c r="C49" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{4.2,1.654},</v>
       </c>
-      <c r="I49">
-        <f t="shared" si="0"/>
-        <v>5.6561704921620659E-2</v>
+      <c r="H49">
+        <f t="shared" si="1"/>
+        <v>4.1929626000000049</v>
+      </c>
+      <c r="I49" s="3">
+        <f t="shared" si="2"/>
+        <v>0.16755714285703113</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -4394,12 +4602,16 @@
         <v>1.6419999999999999</v>
       </c>
       <c r="C50" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{4.4,1.642},</v>
       </c>
-      <c r="I50">
-        <f t="shared" si="0"/>
-        <v>5.6151341887122806E-2</v>
+      <c r="H50">
+        <f t="shared" si="1"/>
+        <v>4.4013798000000079</v>
+      </c>
+      <c r="I50" s="3">
+        <f t="shared" si="2"/>
+        <v>-3.1359090909263442E-2</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -4410,12 +4622,16 @@
         <v>1.631</v>
       </c>
       <c r="C51" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{4.6,1.631},</v>
       </c>
-      <c r="I51">
-        <f t="shared" si="0"/>
-        <v>5.5775175772166445E-2</v>
+      <c r="H51">
+        <f t="shared" si="1"/>
+        <v>4.5924289000000051</v>
+      </c>
+      <c r="I51" s="3">
+        <f t="shared" si="2"/>
+        <v>0.16458913043466308</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -4426,12 +4642,16 @@
         <v>1.619</v>
       </c>
       <c r="C52" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>{4.8,1.619},</v>
       </c>
-      <c r="I52">
-        <f t="shared" si="0"/>
-        <v>5.5364812737668592E-2</v>
+      <c r="H52">
+        <f t="shared" si="1"/>
+        <v>4.8008461000000047</v>
+      </c>
+      <c r="I52" s="3">
+        <f t="shared" si="2"/>
+        <v>-1.7627083333434289E-2</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -4445,9 +4665,13 @@
         <f>CONCATENATE("{", A53, ",", B53, "},")</f>
         <v>{5,1.608},</v>
       </c>
-      <c r="I53">
-        <f>B53/29.2424</f>
-        <v>5.4988646622712231E-2</v>
+      <c r="H53">
+        <f t="shared" si="1"/>
+        <v>4.9918952000000019</v>
+      </c>
+      <c r="I53" s="3">
+        <f t="shared" si="2"/>
+        <v>0.16209599999996271</v>
       </c>
     </row>
   </sheetData>
@@ -4458,15 +4682,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G19"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -4477,17 +4709,25 @@
         <f>CONCATENATE("{", A2, ",", B2, "},")</f>
         <v>{0,1.273},</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2">
+        <f>27.0883-(21.309*B2)</f>
+        <v>-3.8056999999998453E-2</v>
+      </c>
+      <c r="F2" t="e">
+        <f t="shared" ref="F2:F11" si="0">((A2-E2)/A2)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>0.2</v>
       </c>
@@ -4495,11 +4735,19 @@
         <v>1.262</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C13" si="0">CONCATENATE("{", A3, ",", B3, "},")</f>
+        <f t="shared" ref="C3:C13" si="1">CONCATENATE("{", A3, ",", B3, "},")</f>
         <v>{0.2,1.262},</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <f t="shared" ref="E3:E13" si="2">27.0883-(21.309*B3)</f>
+        <v>0.1963419999999978</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>1.8290000000011075</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>0.4</v>
       </c>
@@ -4507,11 +4755,19 @@
         <v>1.2490000000000001</v>
       </c>
       <c r="C4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>{0.4,1.249},</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <f t="shared" si="2"/>
+        <v>0.47335899999999498</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>-18.339749999998737</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>0.6</v>
       </c>
@@ -4519,11 +4775,19 @@
         <v>1.242</v>
       </c>
       <c r="C5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>{0.6,1.242},</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <f t="shared" si="2"/>
+        <v>0.62252200000000002</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>-3.7536666666666738</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>0.8</v>
       </c>
@@ -4531,11 +4795,19 @@
         <v>1.2330000000000001</v>
       </c>
       <c r="C6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>{0.8,1.233},</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <f t="shared" si="2"/>
+        <v>0.81430299999999534</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>-1.7878749999994115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>1</v>
       </c>
@@ -4543,11 +4815,19 @@
         <v>1.226</v>
       </c>
       <c r="C7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>{1,1.226},</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <f t="shared" si="2"/>
+        <v>0.96346600000000038</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>3.6533999999999622</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>0</v>
       </c>
@@ -4555,11 +4835,19 @@
         <v>1.272</v>
       </c>
       <c r="C8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>{0,1.272},</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <f t="shared" si="2"/>
+        <v>-1.6747999999999763E-2</v>
+      </c>
+      <c r="F8" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>0.2</v>
       </c>
@@ -4567,11 +4855,19 @@
         <v>1.2609999999999999</v>
       </c>
       <c r="C9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>{0.2,1.261},</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <f t="shared" si="2"/>
+        <v>0.21765100000000004</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>-8.8255000000000141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>0.4</v>
       </c>
@@ -4579,11 +4875,19 @@
         <v>1.2529999999999999</v>
       </c>
       <c r="C10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>{0.4,1.253},</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <f t="shared" si="2"/>
+        <v>0.38812300000000022</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>2.9692499999999509</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>0.6</v>
       </c>
@@ -4591,11 +4895,19 @@
         <v>1.244</v>
       </c>
       <c r="C11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>{0.6,1.244},</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <f t="shared" si="2"/>
+        <v>0.57990399999999909</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>3.3493333333334818</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>0.8</v>
       </c>
@@ -4603,11 +4915,19 @@
         <v>1.2330000000000001</v>
       </c>
       <c r="C12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>{0.8,1.233},</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <f t="shared" si="2"/>
+        <v>0.81430299999999534</v>
+      </c>
+      <c r="F12">
+        <f>((A12-E12)/A12)*100</f>
+        <v>-1.7878749999994115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>1</v>
       </c>
@@ -4615,17 +4935,25 @@
         <v>1.2250000000000001</v>
       </c>
       <c r="C13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>{1,1.225},</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <f t="shared" si="2"/>
+        <v>0.98477499999999552</v>
+      </c>
+      <c r="F13">
+        <f>((A13-E13)/A13)*100</f>
+        <v>1.5225000000004485</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
@@ -4647,7 +4975,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>